<commit_message>
First mvc architecture, Bug fixes and implemented more features
</commit_message>
<xml_diff>
--- a/Donot_Change/Ticket.xlsx
+++ b/Donot_Change/Ticket.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\Documents\NetBeansProjects\new_mizan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohamed-Tuf-PC\Documents\NetBeansProjects\new_mizan_MVC\Donot_Change\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{487C59A5-BCB7-4756-977A-301EA97A6652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2713496-4A3F-46BA-9553-9206391E4F6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -168,14 +168,20 @@
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -191,12 +197,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -216,9 +216,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -256,7 +256,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -362,7 +362,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -504,7 +504,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -512,7 +512,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:D11"/>
@@ -530,60 +530,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6"/>
-      <c r="B1" s="8"/>
-      <c r="C1" s="4" t="s">
+      <c r="A1" s="8"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="5"/>
+      <c r="D1" s="7"/>
     </row>
     <row r="2" spans="1:4" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="4" t="s">
+      <c r="A2" s="8"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5"/>
+      <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:4" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="4" t="s">
+      <c r="A3" s="4"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="5"/>
+      <c r="D3" s="7"/>
     </row>
     <row r="4" spans="1:4" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="4" t="s">
+      <c r="A4" s="8"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="5"/>
+      <c r="D4" s="7"/>
     </row>
     <row r="5" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="4" t="s">
+      <c r="A5" s="8"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="5"/>
+      <c r="D5" s="7"/>
     </row>
     <row r="6" spans="1:4" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="6"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="4" t="s">
+      <c r="A6" s="8"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="5"/>
+      <c r="D6" s="7"/>
     </row>
     <row r="7" spans="1:4" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="4" t="s">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="5"/>
+      <c r="D7" s="7"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
@@ -626,7 +626,7 @@
     <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.21" right="0.11" top="0.3" bottom="0.45" header="0.04" footer="0.04"/>
-  <pageSetup paperSize="258" scale="91" orientation="portrait" verticalDpi="203" r:id="rId1"/>
+  <pageSetup paperSize="258" orientation="portrait" verticalDpi="203" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"-,Bold"&amp;14الصفا و المروه للغزل و النسيج</oddHeader>
     <oddFooter>&amp;C&amp;"-,Bold"&amp;14وجيه عماره

</xml_diff>